<commit_message>
History page updated. Dates page  updated.
</commit_message>
<xml_diff>
--- a/KM_plakett.xlsx
+++ b/KM_plakett.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://andreslagerlof-my.sharepoint.com/personal/andres_lagerlof_org/Documents/Övrigt/Fäktning/KM/KM_webb/fff_km/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrésLagerlöf\OneDrive - Andrés Lagerlöf Konsulttjänst AB\Övrigt\Fäktning\KM\KM_webb\fff_km\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{ED3410AF-E8C9-459A-94B9-1FF95E490908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{965E1258-E7F8-43CD-BDE5-C0B82B5B1015}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1592459D-6936-4730-B8F5-6889B8246550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{40B36B2C-2698-4287-A7C0-02B2E05705E2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>Year</t>
   </si>
@@ -447,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC9507A-91FD-4CA8-99E8-BC940236C8AA}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -468,55 +468,55 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -524,39 +524,39 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -564,63 +564,63 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
@@ -628,103 +628,103 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
@@ -732,47 +732,47 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>1975</v>
+        <v>1982</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>1974</v>
+        <v>1975</v>
       </c>
       <c r="B40" t="s">
         <v>16</v>
@@ -780,7 +780,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>1972</v>
+        <v>1973</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
@@ -796,15 +796,15 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>1950</v>
+        <v>1972</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="B44" t="s">
         <v>17</v>
@@ -812,15 +812,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>1948</v>
+        <v>1949</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>1947</v>
+        <v>1948</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
@@ -828,25 +828,33 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>1946</v>
+        <v>1947</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>1945</v>
+        <v>1946</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49">
+        <v>1945</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A50">
         <v>1944</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>